<commit_message>
Merge conflicts solved. Reference files updated (redundant diff. styles removed)
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/StyleReferenceFiles/ConditionalFormattingOrder/ConditionalFormattingOrder.xlsx
+++ b/ClosedXML_Tests/Resource/StyleReferenceFiles/ConditionalFormattingOrder/ConditionalFormattingOrder.xlsx
@@ -68,61 +68,36 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="2">
+  <x:cellStyleXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
+  <x:cellXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="常规" xfId="0" builtinId="0"/>
   </x:cellStyles>
-  <x:dxfs count="6">
+  <x:dxfs count="3">
     <x:dxf>
       <x:fill>
-        <x:patternFill>
-          <x:bgColor rgb="FF0070C0"/>
+        <x:patternFill patternType="solid">
+          <x:fgColor auto="1"/>
+          <x:bgColor theme="9"/>
         </x:patternFill>
       </x:fill>
     </x:dxf>
     <x:dxf>
       <x:fill>
-        <x:patternFill>
+        <x:patternFill patternType="solid">
+          <x:fgColor auto="1"/>
           <x:bgColor rgb="FFFFFF00"/>
         </x:patternFill>
       </x:fill>
     </x:dxf>
     <x:dxf>
       <x:fill>
-        <x:patternFill>
-          <x:bgColor rgb="FFFF0000"/>
-        </x:patternFill>
-      </x:fill>
-    </x:dxf>
-    <x:dxf>
-      <x:fill>
-        <x:patternFill>
-          <x:bgColor theme="9"/>
-        </x:patternFill>
-      </x:fill>
-    </x:dxf>
-    <x:dxf>
-      <x:fill>
-        <x:patternFill>
-          <x:bgColor rgb="FFFFFF00"/>
-        </x:patternFill>
-      </x:fill>
-    </x:dxf>
-    <x:dxf>
-      <x:fill>
-        <x:patternFill>
+        <x:patternFill patternType="solid">
+          <x:fgColor auto="1"/>
           <x:bgColor rgb="FFFF0000"/>
         </x:patternFill>
       </x:fill>
@@ -413,14 +388,14 @@
   <x:sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <x:sheetData>
     <x:row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <x:c r="A1" s="1" t="n">
+      <x:c r="A1" s="0" t="n">
         <x:v>10</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:phoneticPr fontId="1" type="noConversion"/>
   <x:conditionalFormatting sqref="A1:A1">
-    <x:cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="greaterThan">
+    <x:cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="greaterThan">
       <x:formula>5</x:formula>
     </x:cfRule>
     <x:cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="greaterThan">

</xml_diff>